<commit_message>
Get daily reddit data: Tue Aug 12 08:13:24 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_17.xlsx
+++ b/data/collected_data/2025_08_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C507"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3508 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1mo2lq5</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>5 star nails I did today</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo2lq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1mo176q</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Can you guys please help me out? Which nail shape do you think suits me best? Thanks</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo176q</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1mo13tc</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Soft, sweet and simple❤✨</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14q3a1m37jif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1mo0yz3</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Berry Sweet Nails 🍓</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y210tioq5jif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1mo0kwd</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Add some sparkles in life</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo0kwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1mo023u</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>My nail lady is amazing.</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5mbm0eawiif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1mnzro4</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Dream-core Gels</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnzro4</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1mnyh35</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>what’s wrong with my nail care</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnyh35</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1mnyruk</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>New Nails for School</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/06fk7lusjiif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1mnykkn</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Gluing Impress Press Ons??</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mnykkn/gluing_impress_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1mnvfch</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Am I being picky?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jwest007rhif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1mnxs72</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>I'm loving these nails 💯</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/227hxokwaiif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1mnwb7y</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Respected nail people of Reddit, I humbly present to you, 6 months of hard work!</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/66cpt4cdyhif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1mnxcb1</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>First Time with Blooming Gel</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnxcb1</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1mnx66w</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Thoughts one Blank Beauty</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://blankbeauty.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1mnwbdw</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Started with a normal polish. Ended up with corn 🌽</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axgzkwueyhif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1mnw8r7</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Just finished making this set today🐍💅🏼</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnw8r7</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1mnw78t</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>butterfly</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6l3kd9cgxhif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1mnw5n7</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bk06gv74xhif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1mnw1oc</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Summer nails ☀️ 🍉🍊🍓🥝</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gj8p1d89whif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1mnvgj0</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Blue polka dots frenchies</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnvgj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1mnumqq</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>What shape nails for my hand type?</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnumqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1mnub9u</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>First time trying black toes</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnub9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1mntrby</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Does this lilac polish suit me?</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mntrby</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1mntm1q</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Painting The Little Mermaid for my nail set display case! Starting with Ariel ❤️</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/61c18e2mchif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1mntjpa</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Help! My favorite neon pink gel polish has been discontinued</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gdhflg93chif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1mnsqq5</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Better on the almonds!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnsqq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1mnsaqj</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>real or fake natural nails……</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnsaqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1mnrwut</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Is it possible to to make my nail stay together after it breaks</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uwv5ivubzgif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1mnrtaz</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>New nails 💕💕😍🥰 Duckies</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65g1dbsxygif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1mnrpky</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Birthday Rococo Nails!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnrpky</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1mnrecu</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>My kid did my nails! (12 YO)</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnrecu</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1mnr58e</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Nail blindness?</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gq5zqpm1ugif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1mnqxe1</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Wedding nails - First time getting nails done!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnqxe1</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1mnqcdx</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>strawbaby</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnqcdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1mnq44k</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>How often do I get it redone?</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecqduq5tmgif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1mnpx15</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>New nail tech did me unbelievably good today</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnpx15</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1mnphoq</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>My nails are changing colours</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lg9223iigif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1mnh23k</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Hashimotoes nails</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mnh23k/hashimotoes_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1mnos8r</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Tried to do vintage ceramic tiles nails</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to3hajesdgif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1mnonw6</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>WHICH DESIGN TO GET FOR PARTY PLEASE HELP.</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnonw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1mnolbo</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Unintentional take on Van Gogh’s Starry Night 🌌</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/oo131zo2cgif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1mnoc1f</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Press on nails for tiny hands...</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnoc1f</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1mnn5xv</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Pedi pain?</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mnn5xv/pedi_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1mnn9jy</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>White spots/bubbles under my builder gel</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnn9jy</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1mnntle</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Too thick?</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dw287na7gif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1mnmtep</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Nail glue recommendations??</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8878edal0gif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1mnmjwz</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>I did my sisters nails. We did a dessert/summer theme</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/repeo2tsyfif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1mnm41q</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>First French I've had done that I haven't been disappointed with</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3vvktpuuvfif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1mnltdk</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>How can i improve</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnltdk</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1mnlj97</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Am I paranoid?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnlj97</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1mnlooh</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Another stained glass set for my cousin!</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnlooh</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1mnll9s</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Why do I have bad ridges and how to fix</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3sjbkohasfif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1mnlfro</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>This weeks color!</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnlfro</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1mnlefw</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>New 🥰</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nb25od1rfif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1mnlbho</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Second time trying isolated chrome!</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnlbho</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1mnl88k</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Which nails for my birthday</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnl88k</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1mnkwbe</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Basic blue for my 30th bday</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k69rl7sjnfif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1mnkivs</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>first time trying fake nails, they're forest mother of pearl butterfly inspired!!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnkivs</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1mnjzvm</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>xeijayi gel polish</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inzz0ieohfif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1mnk06c</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Soft pink cat eye nails</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnk06c</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1mnjhfk</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Gel-X</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mnjhfk/gelx/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1mnje7r</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>First tortoise attempt</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnje7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1mnjcnx</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>First time ever using press-ons</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnjcnx</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1mnj9qy</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>What do you think about my new nails ?</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnj9qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1mnj4w0</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>What is wrong with my nail?</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnj4w0</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1mnim5v</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>If you're able to wear polish on your toenails for extended periods of time (weeks/months), but have smooth, nice, non-stained nails when you remove it...WHAT are your top tips/secrets?&gt;&gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mnim5v/if_youre_able_to_wear_polish_on_your_toenails_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1mnhdnu</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Help finding the perfect base for rosé glazed doughnut nails (out of specific colours)</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnhdnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1mnincr</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>One nail, two moods</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lr84inv59fif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1mnirvf</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Does anyone else have vertical ridges on their nails?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49bu1zby9fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1mnipda</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>What do you think of my new summer nails? I can't decide which side I like better 😂</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hryhtcyi9fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1mnioij</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>She did it again!😍</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnioij</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1mnis6x</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>BEST Rhinestone glue AND BEST 3D Sculpting gel, like the semi solid ones…</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnis6x</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1mnioiq</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>My first set of BIAB nails. Hopeful for long square nails! 🤞🤞</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpc7n3s19fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1mn7slg</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Would this look cute on short nails? [Nails by Stacey Machin on TikTok]</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi3hymxltcif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1mni9fo</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>The pics aren't great but my nails look so good</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mni9fo</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1mnc0km</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>I put the wrong size press ons how to remove fast?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mnc0km/i_put_the_wrong_size_press_ons_how_to_remove_fast/</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1mngjhf</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>why is my powder polish cracking like this?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q4rqqhgveif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1mni0so</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Feeling like a walking strawberry milk latte today ☕🍓🌸</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96sz2oz45fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1mnhyn5</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>new mani!!</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkgeth8q4fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1mnhg12</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>My Birthday Nail Set 💖</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evqa542c1fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1mnhb6d</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>fun fill for a green themed wedding this weekend!!</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9lok5i4h0fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1mnh3ok</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Autumn Basics</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnh3ok</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1mnfcyg</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etllqklineif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1mnfbeh</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Biab set 🍭</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnfbeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1mnewfx</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Products with long wear that don’t require nail shaving?</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9e7jrhekeif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1mneu6w</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>What shape should I have got?</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jrvi5yphieif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1mnemhh</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>I’m a middle-aged man thats started getting my nails done because I kept breaking them and biting them. This is the third time I’ve had my nails done and I’m loving it.</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnemhh</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1mne0gr</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Blue nails!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4lzlckv8eeif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1mndxl3</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Obsessed with this cat eye set 😍</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qandbxzndeif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1mndxcr</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>🖤🤍🩶</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjfbajkmdeif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1mndtwb</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Green Skittle 🌿🦎🌱</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x1wngwiyceif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1mndk1v</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Tarot Nails The Fool, The Magician, The High Priestess</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mndk1v</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1mncwt9</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Fake nails</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgzpkw6b6eif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1mnc18x</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>So cute!</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnc18x</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1mnbl9f</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Pointed almonds or Stiletto? Too long for a guy?</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnbl9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1mnb9eo</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Acrylics with spray colour 💚</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddtu0397tdif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1mnao37</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>No-peel nail polish brands</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mnao37/nopeel_nail_polish_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1mnag6p</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>What is least damaging</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mnag6p/what_is_least_damaging/</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1mnaa3t</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Painted my own nails at home, how did I do? (Ignore the gloves, winter is harsh here)</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1becn6pckdif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1mo2gxx</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Glass Bead technique on Holo Taco magnetics</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yrzz6akqmjif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1mo1iup</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Cat eye nail polish under a microscope</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/x1qnm470rhif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1mo1czr</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>This manicure took way too long 🙈</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo1czr</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1mo0h3c</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>can't recommend: dollar tree gizmo for magnet spinning</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q6ycxyqtziif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1mo0ffz</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>My magnetic offering - now with less mayhem</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uqy8vff40jif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1mnzjgv</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Goodbye, I Scream Nails. Come back soon?</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnzjgv</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1mnzas5</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Recommendations for jelly polish</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mnzas5/recommendations_for_jelly_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1mnynzm</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>finally admitted it to myself and committed. it became an all-nails-on-deck situation.</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnynzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1mnydf4</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>My kids: you stole all the blocks! Me: it’s gotta be done</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bta4dl57giif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1mnxxdo</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Pick your top 5 polishes</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mnxxdo/pick_your_top_5_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1mnxg3f</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>These BKL magnetics!</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/682ew69z7iif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1mnx1on</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Calling this my Mermaid Mani</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m7ml0jpj4iif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1mnwnx0</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Amazing lego magnet spinner</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DNMw8P5xy_Z/?igsh=bTlnYXB1MTdsbWlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1mnwl8n</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Tried XXL tips for the first time, went full galaxy 🌌</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2mj44p2p0iif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1mnwbsq</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Started with a normal polish. Ended up with corn 🌽</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/axgzkwueyhif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1mnvr3e</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Nostalgic computer games time lapse</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hbytcitkthif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1mnvkjv</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>My glass bead setup</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/00z4szncshif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1mnvewa</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Finally got the glass bead effect!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lf2z53h3rhif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1mnvd01</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>I get it now.</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnvd01</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1mnupdg</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>✨️GLITTER✨️ Rainbow</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vzbiq73clhif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1mnu85t</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Vapor wave nail art</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1l72zcaihhif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1mntte2</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Not sure what this counts as but I’m happy with it!</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v7irxx98ehif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1mnt95m</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>queen of rot 🖤🪦🥀</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnt95m</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1mnt0pr</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>ISO pale blue holo</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvou0ma18hif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1mnszd6</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>So fun!</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ll9o6zyq7hif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1mnsj8g</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Newbie asking a possibly silly question. Magnetic polish. Can I get the 5 petal flower effect using non gel magnetic polish? I never seem to see a variation of magnetic designs for non gel polish?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mnsj8g/newbie_asking_a_possibly_silly_question_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1mnsdbn</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>anyone use dashing diva’s chrome powder kit from target?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/128lgsd23hif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1mns0cl</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>We’re All Mad Here</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mns0cl</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1mnroi4</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Looking for a bright periwinkle polish that matches this Chicory flower</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7evsefpfgif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1mnrocx</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Some variations of PfD Eternal Glow</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnrocx</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1mnrlc1</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>This might be my favorite mani I’ve done</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnrlc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1mnr0g5</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Sooooo my Swifties! Where are we getting our TS12 tangerines?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mnr0g5/sooooo_my_swifties_where_are_we_getting_our_ts12/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1mnq9vt</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Not winning any stem awards but this is still pretty! Cirque Colors BAE</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/70il876xngif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1mnp4bd</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Obsessed with Fields of Lavender</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnp3q1</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1mnoph7</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Glass bead</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/Lm962io.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1mnogx7</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Full Lego tutorial (plus full list of parts) for achieving the "glass bead" magnetic effect</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zwkk6yzu7gif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1mnofbt</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Looking for purple magnetic WITHOUT multichrome</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gfr08abbgif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1mnoda9</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Boldly Lacquer?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mnoda9/boldly_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1mnoah4</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Not really into blues normally!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ogel8rreagif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1mno6zy</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>“Are you going to post them online”</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mno6zy</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1mnnd3e</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Showing off some Blurples</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnnd3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1mnn8vc</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Cute polish, terrible formula</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnn8vc</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1mnn8h9</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>You know you’re obsessed when you get into your rental car and the first thing you think is, “The vent is the same shape as my nails!”</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnn8h9</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1mnmz4o</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Nothing beats a good glitter polish</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6bnghi6o1gif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1mnma0s</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Hard Candy Static (1997)</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i668378wwfif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1mnm1gh</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>It’s magic</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnm1gh</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1mnl20n</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>When you have 10 polishes to try, you try all 10!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnl20n</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1mnkz29</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Natural Pink</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uao16t52ofif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1mnku6t</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>My mani for a visit to Georgia Aquarium 💙</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8qzwxa86nfif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1mnkn6j</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Magic in one coat</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mgovie1flfif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1mnkjyt</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Advice to mute / desaturate / tone down a color?</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hw4dy6blfif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1mnk26i</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>🧡new mani 🧡</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnk26i</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1mnk062</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Cracked - Cinnamon Sugar Crumb</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnk062</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1mnjvug</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Appreciation post for Bottoms Up and Minted! 🩵💚</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnjuda</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1mnjbhr</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>My favorite recent manis ✨</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnjbhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1mnj6f2</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>LA Colors jelly longevity/comparable brands</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mnj6f2/la_colors_jelly_longevitycomparable_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1mnj0ov</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>It's so pretty I forgive it for being pink!</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8bs8m5xgbfif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1mnijel</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>my nails accidentally match my controller  🤩</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecy0r2th7fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1mnifj3</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Obsessed with this mani</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gu0drb9s7fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1mnhzha</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Consider me hypnotized</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bs0yz2ht4fif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1mnhzfv</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Need some Thyme off ✈️</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e6a8jvzu4fif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1mnh3rq</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Please help me match my new beads!</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko4mcyy0zeif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1mnguac</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Is there a difference between a matte polish vs a regular polish with matte topcoat?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mnguac/is_there_a_difference_between_a_matte_polish_vs_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1mngs10</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Whirling Dervish 2 Ways</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mngs10/whirling_dervish_2_ways/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1mngnm6</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Don’t be like me: charge your drill before trying to do the glass bead method</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mngnm6/dont_be_like_me_charge_your_drill_before_trying/</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1mnf5l5</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>high grit glass nail file</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mnf5l5/high_grit_glass_nail_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1mnetw3</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>A little disappointed in this PPU polish, was wondering if this happened to others.</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnetw3</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1mndwmu</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Hera* is an absolute queen</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mndwmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1mndvha</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Green skittle</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s0gnv5h9deif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1mndlo2</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Problem with solar polish?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgdr20tebeif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1mndj0v</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Mooncat's Malevolent with a windchime spinner Lego house 😆</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/w9zedyzsaeif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1mndix0</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>Karate nails</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhxtpfnuaeif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1mndbkc</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Over here doing the least 😂 (avoiding magnetics for the moment due to enjoying so many on this sub) But i’m at least using up my collection! i love a mismatch mani and i wanted to use two of my PPU polished i just got.</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mndbkc</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1mncgaw</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>blueberry lemon nails, long version</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xsrxmvs2eif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1mnc9f3</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Excuse my interruption of the spinning magnet madness, but wanted to share this effect!</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnc9f3</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1mnb5hk</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>🌌🌎OUTER SPACE!🪐🌌</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnb5hk</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1mn9bxu</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Glass bead tips?</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mn9bxu/glass_bead_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1mn9824</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Swatch Request: Infinite Thrill</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mn9824/swatch_request_infinite_thrill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1mn8vse</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mn8vse/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1mn7lpw</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Are my nails superdestroyed or semi ok?</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mn7lpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1mn7hts</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Blank Beauty Polish</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mn7hts/blank_beauty_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1mnzb51</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Obsessed with this black cat eye polish ✨</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnzb51</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1mnxofu</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>After &amp; Before...</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnxofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1mnxb66</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Minimal color, maximum charm 🍒</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z2amq1ps6iif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1mnx8nw</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>First time using blooming gel</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnx8nw</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1mnwaqv</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Just finished making this set🐍💅🏼</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnwaqv</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1mnw1ug</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>🍓</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlv0nllawhif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1mnw1az</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Golden nails</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5girswe4whif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1mnvsca</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Loved my Italy trip so much I had to do a nail set for it haha</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hl8gdttwshif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1mntmc2</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Painting The Little Mermaid for my nail set display case! Starting with Ariel ❤️</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ez68e8hochif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1mns6q1</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>nail art advice</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1mns6q1/nail_art_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1mns4hw</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Iron Man coded pressons</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mns4hw</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1mnrzhu</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Red Polish... I'm sorry!</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwn1m6u70hif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1mnrdq2</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>My kid did my nails! (12 YO)</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnrdq2</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1mnqn5h</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Work lately ✨💜</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnqn5h</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1mnqb96</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>strawbaby</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnqb96</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1mnoq88</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Addicted to blooming gel 🙈</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ai2f1fkzcgif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1mnoi6o</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>a classy little gold moment.</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnoi6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1mnnx0v</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Blackpink nails update</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnnx0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1mngkmu</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>just starting out</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mngkmu</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1mnaavz</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>felt lucky 🍀</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mnaavz</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1mn9mwv</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Mix and match set 🐞🐛</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mn9mwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1mn92x0</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I sculpted a shark head for an ocean themed nail set I'm doing</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mn92x0</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1mn8nt2</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Advice please - Jelly polish looks like my nails are dirty at the hyponychium 😬</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/byzz0wem3dif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1mn8fzv</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>new nails</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7gsrxd51dif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1mn83uw</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Made some colorful nails 🌈</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyb8s7r8xcif1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Aug 13 08:13:09 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_17.xlsx
+++ b/data/collected_data/2025_08_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C507"/>
+  <dimension ref="A1:C699"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9052,6 +9052,3270 @@
         </is>
       </c>
     </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1moxk32</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Are my natural nails too long?</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moxk32</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1mowfkk</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Help a newbie out: is this good work?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mowfkk</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1mow26q</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>New to Gel Nails</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mow26q/new_to_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1mow1dy</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Last set for the summer 😊</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9s1mprx74qif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1mouunh</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>First Acrylic Overlay Set</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gcafy5zrpif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1moulo0</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Terrifier nails.</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pllgd8tppif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1mou8ij</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>How about the change? These are my birthday nails.</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mou8ij</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1motthy</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Summer stilettos</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bwkopz6iipif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1motooe</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>🕷Acrylics</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1motooe</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1motmyl</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Graduation nails ✨️💚</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pghfuk7vgpif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1mosy6m</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Reputation inspired nails</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzcwpaawapif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1mostzp</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Ideas for fall nails</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mostzp/ideas_for_fall_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1mos2uz</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Swirlies!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mos2uz</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1mos70b</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>New nails for the last month of summer</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7qilp7j4pif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1mos0z9</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Purples! 💜</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mos0z9</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1morshj</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>inspired by Merlina 🖤🤍</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu3e9pox0pif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1morpnc</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Studio Ghibli inspired set</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1morpnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1moqnxe</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Before and after shaping my nails</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moqnxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1moqrm8</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Before and After shaping my nails</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1moqrm8/before_and_after_shaping_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1mormwl</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>What to do about broken nail?</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ogap71hszoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1morlgv</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Simple Leo design</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eofyn30hzoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1mor9cb</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Nude color with white French</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zg69isnwoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1mor0lu</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>🦄Opal and gold set</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhb5z3xmuoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1moqwwz</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>tequila and lime 🍹🧂🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moqwwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1moquqo</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>I love how the cuticles turned out! Although I think they are a little long</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7syx7p1froif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1moqeho</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Iron Man ❤💛 Pressons</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0vi8taqmpoif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1moqemb</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>So fun to design!</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vedhblhppoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1moouid</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>medieval fantasy nail set i did!!</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moouid</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1mooqnm</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>She’s beauty, she’s grace, she’s… an emoji 💅🏼😂</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mooqnm</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1monzu9</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>First try 🍉🫐🍓🍋</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/13m2zcsd6oif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1monpyb</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Nails for the month of August :)</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1monpyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1moni27</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Black and green cateye</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xy3vapt23oif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1moluc7</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Cat Claw Girlies - How are they?</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1moluc7/cat_claw_girlies_how_are_they/</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1mon5ld</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>The only set of nails I’ve ever done (they were so pretty but I love my natural nails too much to do it again)</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mon5ld</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1momxik</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Apres Nail Tips</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1momxik/apres_nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1momx2s</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>This or That?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1momx2s</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1momah3</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>DIY press ons using softgel full tips and cat eye polish -  applied with sticky tabs! Much stronger and harder than any press on I’ve bought - I made 2 sets for my trip</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1momah3</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1mom5qb</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Red chrome to end the summer!</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cl5kk3odtnif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1molrva</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Practicing with dual forms and poly/sculpting gel 🥰 thought they came out cute</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1molrva</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1mollx2</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Cat eye has us all in a chokehold, huh?</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wmt3mugkpnif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1mol8id</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>My nail art 🩷🩷🩷</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mol8id</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1mol1hl</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>I’m 21 but this is my first time getting my nails done at a salon! (I wanted a dark mcbling, 2000s inspired look)</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/petdhz2qlnif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1mokroq</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>I don’t know if this is the right place for this, but this ALWAYS happens to my nails when I try to grow them out long. It’s so frustrating. What can I do to fix this or prevent it from happening?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mokroq</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1mokr7m</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>How do you guys whiten your nails?</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypvf9p0tjnif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1mojvvd</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>I adore my new nails. Recent ones in photos too</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mojvvd</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1mojr66</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>My cutesy pink marble mani.</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mojr66</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1moiti3</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Here is my recreation of this set😁</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moiti3</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1mois95</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>My first Biab ✨❤️</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6qq82rjo6nif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1moio7t</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Bet you can’t guess who this client is going to see?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4u6hhcox5nif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1moik4d</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Post COVID self care</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moik4d</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1moig2y</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Disadvantages of gel nails</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nrnnv83f4nif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1mohy9p</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>How does one shape a square nail?</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mohy9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1moh64m</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Are press ons supposed to sting?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moh64m</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1mogsvz</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>i adore my nail artist 💖</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mogsvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1moez58</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>should i be concerned about my pinky?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/roo3sduyhmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1mogl3z</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>My first time doing my own acrylic nails!</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnmxu65bsmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1moghal</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Blueberry lavender cat eye and chrome combo</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xbnko3jmrmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1mogf3x</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Plants and nails my favorite things! 💕💕💕</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmhzwv48rmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1mofry2</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>A fun pop of colour for the summer!! 💖</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mofry2</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1mof8fn</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Molten Shells 🐚</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6whx4n1njmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1mof350</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Just started doing my own polka dots. Not the best, but I like them</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ut29luoimif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1moezz5</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>First time getting my nails done ❄️🤍</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/up4m8hj4imif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1moeh4t</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Are these nails weird in a good or bad way?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4plxqrwnemif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1moe65t</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Where to find nail inspiration when Pinterest is full of AI and ads? 😕</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1moe65t/where_to_find_nail_inspiration_when_pinterest_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1mo1gh8</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Toenails still thin and brittle after two years of growth</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mo1gh8/toenails_still_thin_and_brittle_after_two_years/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1moe0ja</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Is it time for a fill or can I wait another week?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hg316etobmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1moe0hr</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Cuticle and apex help!</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moe0hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1modx1d</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>throw back to when i did my valentines nails 💋</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hm219492bmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1mo95y4</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Finally attempted some designs on my own!</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo95y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1mo87ik</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>New regular nail polish user</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mo87ik/new_regular_nail_polish_user/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1mo9owu</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>PSA: be cautious of the chemicals in gel polish</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo9owu</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1mob6i2</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Advice (gel keeps peeling off) PLEASE🙏</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lwz0jvcuslif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1mob8p1</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Should I be pleased with these nails</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mob8p1</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1modco7</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>I make my own press ons (just for myself)</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rc754g9d7mif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1mod79h</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>My natural nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vjf90b3e6mif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1mod73s</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>I’m a dragon!</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mod73s</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1moct5z</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>I match my nails to my cosplay. This time purple catseye</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ejvknwk3mif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1mocove</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Anyone know how I can fix my nail?</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mocove</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1mocib6</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Coffin or almond nails?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mocib6</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1mocech</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Beginner Gel X set</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l53q6po21mif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1mocdm5</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Summer yellow</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mocdm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1mobygt</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>summer sets 💓</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mobygt</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1mo9tze</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Anxiety nail biting (extreme?) - any tips on how to repair</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo9tze</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1mo9bn4</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>I am so impressed by my new nail tech!!!</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo9bn4</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1mo7s07</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>Pogo The Clown Nails</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/twd9c6cg4lif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1mo7bs4</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Gel x or wait?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0cogb4v0lif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1mo72vf</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0fhu24tykif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1mo6uuf</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>What do you think of my ombré set I just got for this week?</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29e7n8wvwkif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1mo6lnn</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>Biab vs acrylic</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mo6lnn/biab_vs_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1mo6grl</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Tips on how to apply chrome powder better?</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mo6grl/tips_on_how_to_apply_chrome_powder_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1mo68zu</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>I  swear nail polish never dries on my nails and I have no clue why.</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mo68zu/i_swear_nail_polish_never_dries_on_my_nails_and_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1mo5qm0</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Butter nails 🧈 💛</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8eghyvumkif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1mo4iqk</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I cant remove the dual form</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mo4iqk/i_cant_remove_the_dual_form/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1mo3orn</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>What nail shape should I go for i know they aren't very long</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mo3orn/what_nail_shape_should_i_go_for_i_know_they_arent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1mo3mc8</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Engagement nail ideas please</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mo3mc8/engagement_nail_ideas_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1moy1nl</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Hmm, not sure about this one</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moy1nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1moxi16</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>pls tell me what other polishes have magnetics with super fine particles!!</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/65yzppnwjqif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1mox6n5</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Leo ♌️ Whatcha Indie Polish</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ijbd5ligqif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1mowy90</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Just received my first Clionadh cosmetics order 🤤</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qrfxq7xrdqif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1mow9ai</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>New fave!!</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mow9ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1mow4wx</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Nail stickers!</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mow4wx/nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1movlco</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>for my canadian lacqueristas - inspiredsense</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1movlco/for_my_canadian_lacqueristas_inspiredsense/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1move3z</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Got the lab stirrer 🥴. Y'all.</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1move3z</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1mouigt</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Just here to deter anyone from impatiently ripping your nails off. Don’t be like me.</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhjxva7zopif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1mou92s</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Soft Summer Vibes</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mou92s</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1motq4r</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Good Base Coat?? Excluding Orly Bonder</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1motq4r/good_base_coat_excluding_orly_bonder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1motdcb</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Silly question- how to tell if your nails are soft vs brittle?</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1motdcb/silly_question_how_to_tell_if_your_nails_are_soft/</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1moszgf</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Accidental skittle</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moszgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1moscgq</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>I feel silly having to ask this</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1moscgq/i_feel_silly_having_to_ask_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1moru9w</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Let’s talk silk wraps</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1moru9w/lets_talk_silk_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1morkzw</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Had a dream about a really interesting polish and now I'm curious if it exists, or is even possible</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1morkzw/had_a_dream_about_a_really_interesting_polish_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1morkm9</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Mooncat Magnetic Mutiny</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1morkm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1mor6ax</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Issues with beyond polish shipping?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mor6ax</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1moqk4d</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>What is the prettiest bottle shape/packaging of nail polish you own? As far as I know nothing beats the Sally Hansen Diamond Strength line</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikft26pyqoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1moqd5m</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Tariffs, no tariffs...yet price increase is here to stay?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qa76gv7dpoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1mopswi</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>New Sally Hansen topcoats</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mopswi/new_sally_hansen_topcoats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1mopkud</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>ILNP ECLIPSE 🥀</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2o5dzvgiioif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1mopafw</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Baby’s first thermal</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mopafw</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1mop0b1</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Light reflective polish under microscope</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7gjymsfeoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1moo1ed</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>sprung forth ✨</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moo1ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1monyqc</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Mixing madness!!</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2th4aath6oif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1monuj3</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Sometimes you just need to have a pink palate cleanser 💖</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1monuj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1monm3v</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Favorite polishes with subtle/delicate holo?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7rqn8xy3oif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1mon754</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Magnetic French tips ✨</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mon754</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1momsmh</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>In love with my fish nails!</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1momsmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1mom943</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>What do we think of these Cupcake polishes?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/de2xeer2unif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1molpnc</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Recommend your favorites!</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1molpnc/recommend_your_favorites/</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1molcij</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Matched my eyes to my polish</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1molcij</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1mokbdq</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Added a £10 motor to some spare Lego I had lying around.</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvddv2rugnif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1mok98u</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>homemade cuticle oil for nail growth?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mok98u/homemade_cuticle_oil_for_nail_growth/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1mojia4</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Can you guess what "special effect" nail polish this is supposed to be?😭</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mojia4</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1moitms</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Norpsilocin ft. my fav hand model</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moitms</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1moiskw</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>New indie brand alert! Snacker Lacquer launching 8/22!</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moiskw</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1moik4w</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Gamer Polish</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vki0fpj65nif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1mogzt6</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Anyone have swatches of Forge by Clionadh?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mogzt6/anyone_have_swatches_of_forge_by_clionadh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1mogxj3</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Seasonal laqueristas: When do y'all switch to "fall" colors??</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mogxj3/seasonal_laqueristas_when_do_yall_switch_to_fall/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1mogqxi</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Glitter gradients are tough 😬</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mogqxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1mogirk</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Where can I find sequins like this?! HELP</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qq7o31awrmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1mogfjw</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>My 90s inspired electric feels and pastel dreams</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/Klc229f</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1mogdfo</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Opi comparison</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yk8gbbhxqmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1mogbn1</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>my new polishes im hyped on</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mogbn1</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1mog59r</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>Ordering Cadillacquer</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mog59r/ordering_cadillacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1mog2xg</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>I am dead inside 🫥</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2f4fqy1pmif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1mofpgm</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>A fun pop of colour for the summer!! 💖 {Gifted PR}</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mofpgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1mofdw0</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Experimented layering ILNP Lily in velvet effect with Fairy Dust ✨</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mofdw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1moenq4</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Bee’s Knees vault is empty?</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1moenq4/bees_knees_vault_is_empty/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1moebdo</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Probelle nail concealer and a question</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moebdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1modne5</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Perfect neutral for a cool olive tone</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1modne5</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1modhmj</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>MILF (Multichrome in Lacquer Form)</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gksoqxs88mif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1mod002</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Peel Off Basecoat Recs?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdsm6sf25mif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1mocvwz</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Does speed matter?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/culebjv44mif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1mocmot</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Acidic Tears by Cracked</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kqwjarjm2mif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1moc8ol</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>My orange and green Taylor Swift-inspired nails</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qbesmkl10mif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1moc5st</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Holo Taco Cloud Nine🩷</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzs2fx3izlif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1moc44v</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Ugh, I’m so bummed 😭-dupe request?</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnbiy6s6zlif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1mobd43</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>This shade is a dream</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tlpgxuh4ulif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1mobbe6</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Stripe magnet</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b2sq3ulstlif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1moag78</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>slightly overfiled my nails</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ll8fh9vwnlif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1moa4u5</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>In need of top coat advice!!!</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1moa4u5/in_need_of_top_coat_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1moa4e0</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Shade Name? 🌸</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moa4e0</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1moa1dj</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Should I be cleaning residue off of my top coat bottles?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1moa1dj/should_i_be_cleaning_residue_off_of_my_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1mo9iom</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Favorite polish and/or color on short nails?</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9qx3a92ghlif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1mo93g1</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Topper tryouts</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo93g1</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1mo8w8v</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>Loving the Mooncat Star Wars collection 🥰</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1ncxsg1wclif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1mo7otr</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Iris inspired</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo7otr</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1mo71t5</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>I completely get the hype now</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo71t5</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1mo715w</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Need a little Mood Boosting ( Feat Central Park )</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo715w</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1mo6yfp</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>If you could call a maker up, and say "Please make this exact polish" what would it be?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mo6yfp/if_you_could_call_a_maker_up_and_say_please_make/</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1mo6w6a</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Mooncat Sin Eater</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo6w6a</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1mo6mk9</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Cirque magnetics are just… 😻</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aahk0hlzukif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1mo6fpp</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Help finding which polish can give off this color</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ej6me5h6tkif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1mo5t7b</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Do you have info about this polish?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo5t7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1mo4ea7</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>New favourite combo!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo4ea7</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1mo4acp</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>What are these patches in my gel polish?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo4acp</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1movfzv</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Purple set</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1movfzv</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1mov1d0</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Last summer nail of the season</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mov1d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1mot7ua</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>a little color 🌈</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mot7ua</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1moq6ki</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Kpop demon hunter set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yqnuhacunoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1mooi8k</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Cateye and chrome</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8663guiaoif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1momudr</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Any advice for what to get my girlfriend who’s into Nail Art</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1momudr/any_advice_for_what_to_get_my_girlfriend_whos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1moksnv</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>the set that made 3d flowers click for me.</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moksnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1mojzw4</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Is anyone here an anime fan?</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yysbdmb8enif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1mojraq</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>why is my top coat bumpy and lacking shine?</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/j0uryfp3dnif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1moij9r</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Merlina-inspired nails 🖤</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ij71zwjp4nif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1mohvg5</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Un poco de arte en 3D</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9io0cxxl0nif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1moe5ap</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Gem sourcing help</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moe5ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1mob2zz</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>a little nail art</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nmk03cu5slif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1mo9a1c</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>End of summer nails created by me!</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3erj2zpoflif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1mo6y83</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Y2K nostalgia nails</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo6y83</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1mo6u38</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Werms 🪱</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jreuiraqwkif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1mo5l4w</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>What nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mo5l4w</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1mo40op</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Ibiza Final Boss nails 🏝️🍹🙈</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5s6r89hu4kif1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Aug 14 06:54:03 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_08_17.xlsx
+++ b/data/collected_data/2025_08_17.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C699"/>
+  <dimension ref="A1:C886"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12316,6 +12316,3185 @@
         </is>
       </c>
     </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1mpt6xi</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Finally managed to grow my nails out a little after years of brittleness 😁</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpt6xi</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1mp0ca5</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>I can’t tell if i love it or hate it</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp0ca5</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1mpdc73</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Birthday set ✨</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpdc73</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1mpr8p2</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>My birthday nails!!! Love love loveee</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5nqdy7b63xif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1mpsf5c</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Allergies?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qk6jzbkxexif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1mpsiyq</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Soft pink Ombre💅💖</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w71hzmofxif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1mpshb0</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>My most recent nails 🍒</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmfcfebjfxif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1mprvtq</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/avi2uycj9xif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1mprhtz</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>My new set</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jyxov60o5xif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1mprcmh</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>🦋Blue Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6saubhc84xif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1mpr3bs</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>bejewled nails</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpr3bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1mpr2s8</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>elegant / ballpit nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpr2s8</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1mpqo87</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Natural nails painted black</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/if5jyj4pxwif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1mpqnfk</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Recent nails I did 😛</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpqnfk</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1mpo7rw</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>How do you guys deal with a bad experience?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpo7rw/how_do_you_guys_deal_with_a_bad_experience/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1mpqc58</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Total beginner question (sorry if this is dumb) about using gel polish</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpqc58/total_beginner_question_sorry_if_this_is_dumb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1mpqgyp</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>2 of my favorite sets!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpqgyp</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1mpfahq</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>should i go for something similar?</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gquqz8q5huif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1mpbno7</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>My nails inspired by Dua Lipa’s manicure</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpbno7</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1mpqali</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>My stiletto nails always dull - what can i do to keep them sharp?</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwajdg31uwif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1mpq93f</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Trouble finding press ons to fit</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpq93f/trouble_finding_press_ons_to_fit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1mpplqo</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Birthday nails 💖💚</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpplqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1mppi9g</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Natural lenght 🫠✨</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f8jacrtmwif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1mpper0</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Duck Nails</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpper0/duck_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1mpp6ba</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Nails for my bachelorette party</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/441s5ldujwif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1mpog83</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Vacation nails🌊🏝️🐚💜 my inspo for these nails came from @chaki.17 on insta!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpog83</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1mpoe1h</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>my first time!!</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/znlh4av0dwif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1mpo9qu</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Tried a new nail salon in town</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/caukp2i0cwif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1mpn4tm</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Travelling to Japan soon and going to get my nails done, need inspo!</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpn4tm/travelling_to_japan_soon_and_going_to_get_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1mpnzvl</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>BIAB after 1 month of growth</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2ipp9yo9wif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1mpnthz</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Rate the color from 1 to 10</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sh4rs0w78wif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1mpnq30</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Do you think I should go back to these for the holidays or Valentines?</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqxon27f7wif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1mpnbpl</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Is chocolate my color?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yhl0i6h64wif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1mpkpv5</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>in love with these nails</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iknxz5wejvif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1mpnaxs</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>No idea how to take photos, wanted to share a gel set I did on a friend tonight 💙</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpnaxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1mpna8m</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>My current duck nails. The rings add balance. 💕💕💕</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3ipr7bv3wif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1mpn8nq</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Any recommendations for good quality gel nails Brand ?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpn8nq/any_recommendations_for_good_quality_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1mpmrgp</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>French Tip acrylic nails with happy shinyness no body sneeze or we've got glitter everywhere</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpmrgp</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1mpmmro</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Birthday set</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xxumsziyvif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1mpmai1</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Acrylics ✨️🐆</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4qicxwysvvif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1mpkn3c</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>First time paying for nail art, is it well done?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nkfjo5c5ivif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1mpl9lc</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>3 hours and I couldn’t say anything but, “ya, they look great” 😭</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwuzxw9mnvif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1mpkzhx</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Press Ons and Builder Gel?</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpkzhx/press_ons_and_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1mpka60</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Gel Nails keep chipping after 3 days</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/157nhvizfvif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1mpk20o</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>these looked cuter holding iced coffee</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dudfn9iaevif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1mpajf7</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Glue tabs plus nail glue - what happens when both are used together?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ie6p9nsltif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1mpfkeh</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Is it too early for fall themes alr?</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpfkeh</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1mpizhi</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Which opi nail colors are these?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/97zm6q6n6vif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1mpagpt</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Welp, it got me</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpagpt/welp_it_got_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1mpbchk</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>New to nail oiling, do I trust this thing to be in my purse?</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8yyp752rtif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1mpck36</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>PLEASE HELP! I NEED TO GET THESE CURRY STAINS OUT OF MY ACRYLICS</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpck36</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1mpiz1g</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>growth</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpiz1g</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1mpjebk</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>last minute set before coffee and errands and no i can't stop staring at them</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b7v7c9zk9vif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1mpj26e</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Obsessed</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpj26e</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1mpj1pp</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>I got my nails done for the first time today✨</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpj1pp</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1mpj0ie</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>beginner to getting nails done- is this normal, or something they should fix?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpj0ie</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1mpiy2n</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Obsessed with my birthday nails 😍. I was hesitant to try the jewels but so happy I did 🥰</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g27wttdd6vif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1mpixww</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Please help— cannot get my acrylic nails off</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpixww/please_help_cannot_get_my_acrylic_nails_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1mpit55</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Some recent manis 💅🏻</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpit55</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1mpigj8</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Atomic Polish - Radon</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpigj8</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1mpiai4</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Tried blooming gel for the first time 🫣</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpiai4</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1mphxlb</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>First time using claw nail forms. I'm hooked.</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ygnm2n7zuif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1mphauq</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Weeknd Ready! 🖤</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80xz5ziuuuif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1mph8rp</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Gel or acrylic?</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mph8rp/gel_or_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1mph4ks</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Did I do a good job applying these press ons? Please ignore the bits of glue lol I will remove that later</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mph4ks</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1mpgxwm</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sw9x81lcsuif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1mpganr</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>OPI Strawberry Margarita 🍓</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pn33cxiwnuif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1mpg598</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Toetally bummed..</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpg598</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1mpfv88</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>suggestions</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vn1x8jy0luif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1mpfv66</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Look girls, how did my aunt's nails look?</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0rr242wzkuif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1mpfspp</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Am I being too picky?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpfspp</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1mpfm7j</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>new nails!</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpfm7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1mpfc7n</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>pulling out my swiftie card today 🧡</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpfc7n</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1mpev21</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Little Y2K moment 🩷</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sc6xgroaeuif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1mpeolw</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>I've never had my nails done before, would like advice</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6aegw6r4duif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1mpe9ri</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Normal Nail Growth for 10 Days?</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5amq4kdauif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1mpe9qm</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>My last summer set of the year: Strawberry Picnic!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ci31t1wcauif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1mpe38z</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>I loved them 😍😍😍</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f432hz59uif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1mpdakt</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>I Have Two Questions:</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mpdakt/i_have_two_questions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1mpcw39</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Are these to flat? Just got them done by a new tech yesterday and I've never had such thin/flat nails</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpcw39</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1mpcqar</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Hard gel keeps lifting</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpcqar</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1mpcq6k</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Hard gel keeps lifting</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpcq6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1mpcjj2</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>What do these white lines mean?</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tb01sryuytif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1mpc8ut</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>What would you add?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7kw64zzvwtif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1mpc5b1</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>I think it's time to change this green animal print</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2fnzkqa8wtif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1mpb5ac</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Got a manicure at salon, are my expectations too high?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpb5ac</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1mpb2i8</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>New nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/klokdx3aptif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1mpab5h</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>going back to school to finish my degree after 3 years as a full-time nail tech :)</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odv212yaktif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1mp9xu2</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>testing how pink looks on me!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp9xu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1mp08cz</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Circuit Nail Foil?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu3ii3zbfrif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1mp9j6x</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Good press-on brand for low apex?</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mp9j6x/good_presson_brand_for_low_apex/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1mp8u6o</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>simple polka dot bee nails 🐝</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp8u6o</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1mp5a5q</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Feelin’ pretty blue today but that fueled my inspo, prob one of my fave sets to date</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6o3vdl9fmsif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1mou8vm</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Should I keep brittle nails bare or put builder gel on them?</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mou8vm</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1moug3t</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Regrowth gap 1 week after gel manicure</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/awvqri1bopif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1mov5wv</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Petri dish nails</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mov5wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1mp4c59</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Can I put on regular nail polish over my nail that has the green thingie?</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mp4c59/can_i_put_on_regular_nail_polish_over_my_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1mp4h83</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>I’m looking for a UV press on gel glue that also comes with a good remover.</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mp4h83/im_looking_for_a_uv_press_on_gel_glue_that_also/</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1mp8cgz</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Why do I always regret every design I get done</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hikbasaf7tif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1mp7o2f</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Sally Hansen Hard as Nails is Yellowing</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1mp7o2f/sally_hansen_hard_as_nails_is_yellowing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1mpqrca</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>I just feel the need to show of these linear holos</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpqrca</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1mpq3ly</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Plead help me find!</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpq3ly</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1mpq1pm</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Help ID this OPI?</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y2yz0xskrwif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1mppwx4</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Londontown Kur Perfecting Nail Veils without base coat?</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mppwx4/londontown_kur_perfecting_nail_veils_without_base/</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1mppqse</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Supergiant from Fancy Gloss</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mppqse</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1mpphzp</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Noob question: how do y'all get good edges</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpphzp</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1mpowxt</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Canadian Magnetics?</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8q0ltclkhwif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1mpoco8</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Switch Pages- Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpoco8</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1mpoa4w</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>this combo is everything 😍</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ehuz2vi3cwif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1mpnmqd</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Nails match my rain jacket :) 💧🦋🩵</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pozaor4p6wif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1mpnlt6</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Anyone gone from DD to gel?</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vl5b8xwg6wif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1mpmshn</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Water logged nails</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpmshn/water_logged_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1mplkj4</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>When life hands you lemons</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/be7c5p30qvif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1mplk8l</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Nails from a chronically online millennial</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hzz181ypvif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1mplc2b</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Get Lobstered!💜🩵💚</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mplc2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1mpksei</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>As a mechanical engineer I had to make my own setup!</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z8dq4u9sivif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1mpk7lg</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Your favourite Glow in the Darks?✨✨</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpk7lg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1mpk494</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Need tips for destashing. Wanting to sell some of my polishes!</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpk494/need_tips_for_destashing_wanting_to_sell_some_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1mpjsrk</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Examples of a workable formula?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpjsrk/examples_of_a_workable_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1mpjpxv</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Any Canadians Order from Polished for Days lately?</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpjpxv/any_canadians_order_from_polished_for_days_lately/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1mpja5x</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Magnet Stirrer havers, how do you do it?</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpja5x/magnet_stirrer_havers_how_do_you_do_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1mpj4di</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>How do you store magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpj4di/how_do_you_store_magnetic_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1mpj1wy</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Fairy Dust over Sweet Tooth 🧚‍♀️🍭✨</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpj1wy</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1mpiy7b</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Has this happened to anyone else? My nail broke off at the tip but my polish stayed intact 🤨</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8a48dae6vif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1mpiq9l</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer Ocean Water and Force is strong</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpiq9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1mpik0k</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Is it just me, or do you also want pigmented magnetic toppers?</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpik0k/is_it_just_me_or_do_you_also_want_pigmented/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1mpifk8</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Atomic Polish - Radon</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpifk8</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1mpia4d</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>To Celebrate TS12</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsi95w6n1vif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1mpi33t</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>MoonCat nail polish suggestions??</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>/r/mooncatpolish/comments/1mpi0px/mooncat_nail_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1mpi0f0</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Does anyone know a good uv gel match for these two DND colors?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpi0f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1mphe3u</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Showgirl Pre-Pre-Order Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mphe3u</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1mpggag</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Mystic Nail Polish - Sirens Curse</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5xv03fyyouif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1mpg3mv</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>🍎🍂 Painted Polish Mystery Crelly Vingt-Trois 🍁🍏 It's like an an autumn apple orchard in a bottle!</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpg3mv</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1mpfjvx</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>skye velvetized 🩵⛅️</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pzaw4xwxhuif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1mpew0c</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Shopping my Collection</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/z07ctrviduif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1mperyn</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>How to achieve swirly magnetization like this pic?</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvw18klqduif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1mperjw</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>My heart cannot take this kind of excitement!!!</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4139m8tlduif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1mpdrcr</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>BKL magnetic #2: Heartbroken</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpdrcr</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1mpdasj</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>ILNP FlipSide with the Spinning Magnet Technique is INSANE!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/71yqop8u3uif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1mpcyf6</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>I guess I’m a neon person now</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/miu5s8bl1uif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1mpc689</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>How would you approach this?</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x9hhijqewtif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1mpbzlz</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Cut nail a little too close to nail bed, should I still oil the nail ?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/58sl5aw7vtif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1mpb9a8</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>I love to paint my nails to match my projects</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/79cgn3mhqtif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1mpb3do</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>The Life of a Showgirl inspired mani ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90r1ih3gptif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1mpazl0</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>How to make polish stay on nail</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpazl0/how_to_make_polish_stay_on_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1mpaosw</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>PSA: Bee’s Knees Lacquer’s Make Your Brother Proud doesn’t look like this irl (but is still so pretty)</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/m2ou39oqmtif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1mpaoo1</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Autumn’s coming up, what are y’all buying/wearing?</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mpaoo1/autumns_coming_up_what_are_yall_buyingwearing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1mp9faz</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>Can someone please tell me what these are used for?</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kk1fvcnietif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1mp8yvo</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Feeling like an eleven princess in Cracked "Spring Sprout" 🌱🧝🏻‍♂️</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yryqfj4l9tif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1mp8iik</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>PPU Rewind- Daughters of the Evening</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp8iik</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1mp8ca5</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Help with lifting</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp8ca5</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1mp82vn</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Help me decide on my beach nails! bc i am indecisive lol</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2yukeu2m5tif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1mp7t9f</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>my new favorite pink magnetic!!</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vfw131au3tif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1mp76dw</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Recommendations for korean/ japanese style polishes &lt;especially magnetics&gt;</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mp76dw/recommendations_for_korean_japanese_style/</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1mojw5c</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>best and safest way to do nail extensions at home?</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mojw5c/best_and_safest_way_to_do_nail_extensions_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1mobbfo</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Need my polish to endure a lot</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mobbfo/need_my_polish_to_endure_a_lot/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1mp6l03</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>What's your most used bkl magnetic?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mp6l03/whats_your_most_used_bkl_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1mp5lxt</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Took 10 days off work (RN) and the lack of hand sanitizer has done wonders for my nails. How do I keep them this healthy when I go back to using hand sanitizer 200x a day and can’t oil them at work? Are there any treatments I can do? (nails are always painted at work)</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pulb4mloosif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1mp5bj7</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Magnetic polish newbie</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mp5bj7/magnetic_polish_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1mp58hf</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Anyone else attracting wasps this year?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mp58hf/anyone_else_attracting_wasps_this_year/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1mp54lj</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Any pressure on my nailbeds hurts after stopping biting</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mp54lj/any_pressure_on_my_nailbeds_hurts_after_stopping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1mp4vpv</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Peel off base works on teabag nail repair 🤗</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rehu7rmjsif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1mp3rrc</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Looking for stickers like Cirque Colors Gourmand Collection - I'm almost out of my sheet and I would really love to find more like this but they don't sell it anymore!</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp3rrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1mp297g</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>What is this tool?</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp297g</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1mp25g2</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>So, so close! Inspo vs result</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qd1nmp15yrif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1mp1ag7</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Nail cuticle oil pen feels impossible to refill?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp1ag7</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1mp0t5c</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Press-ons for hardworking hands?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1mp0t5c/pressons_for_hardworking_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1moytg6</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Holy grail hand creams for Aussies?</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1moytg6</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1mpsr5y</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Today's work, something simple but tender</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pjov7a3cixif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1mpo0us</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Wanna Get Back Into It 🥺</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fa3gxvhx9wif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1mpnwkl</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>WHEN I WAS BIG INTO DOING NAILS</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/45347d8x8wif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1mpnabp</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>No idea how to take photos, wanted to share a gel set I did on a friend tonight 💙</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpnabp</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1mpn892</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Just wow</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hfdybbgf3wif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1mpn5dt</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>I loved these nails. A friend did them for me.</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2zcpzyr2wif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1mpmb7s</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Acrylics 🐆✨️</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2rl9k52zvvif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1mpj9v4</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Chappell Roan Nails Size L</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mcvw0bp8vif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1mpej0p</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>My jobs today, I love what I do</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpej0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1mpcvbb</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>I need feedback.</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpcvbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1mpbewe</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Summer feel :)</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8l93acirtif1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1mpa0pm</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>I think I have to marry my tech…</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mpa0pm</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1mp9ox2</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Doodle nails ✏️</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp9ox2</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1mp5v5t</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Neon drips</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp5v5t</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1mp4ql6</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Some blooming gel nails vs inspo (last 2 slides)</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp4ql6</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1mp3ev9</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>loved these rockstar inspired nails i did.</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp3ev9</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1mp1gql</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Hehe, I’m back! This time it’s Tanjiro’s little sister, Nezuko!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v8apw3e4rrif1</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1mp1dl8</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Black + glitter ✨️</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6diddu0rrif1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1mp1csd</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Blue stiletto nails 💙🩵</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1mp1csd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>